<commit_message>
all import and export fix
</commit_message>
<xml_diff>
--- a/public/templates/template_aset_kendaraan.xlsx
+++ b/public/templates/template_aset_kendaraan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bismillah_sip_aset\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C4C7E0-F293-41EF-B0CB-2C0ADCA2C010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86CC037-D98C-4EB9-AE52-4EABE42C8652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{4CBD18AC-1254-4C8F-9B02-8616AC47CBCC}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>id_status_aset</t>
   </si>
   <si>
-    <t>kode_aset</t>
-  </si>
-  <si>
     <t>nama</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>Tersedia</t>
   </si>
   <si>
-    <t>02.03.MT.1995.0001</t>
-  </si>
-  <si>
     <t>Sepeda Motor</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t>Honda</t>
   </si>
   <si>
-    <t>C86 solo</t>
-  </si>
-  <si>
     <t>Hitam</t>
   </si>
   <si>
@@ -105,9 +96,6 @@
     <t>GGE-1021671</t>
   </si>
   <si>
-    <t>R 9809 BH</t>
-  </si>
-  <si>
     <t>22/11/2006</t>
   </si>
   <si>
@@ -117,44 +105,26 @@
     <t>Bantuan PEMDA Banyumas</t>
   </si>
   <si>
-    <t>02.03.MB.2005.0001</t>
-  </si>
-  <si>
-    <t>Mobil</t>
-  </si>
-  <si>
-    <t>Mitsubishi</t>
-  </si>
-  <si>
-    <t>L 300 Wagon</t>
-  </si>
-  <si>
-    <t>Biru Metalik</t>
-  </si>
-  <si>
-    <t>MHML300DB5R2399971</t>
-  </si>
-  <si>
-    <t>4D56C-A96302</t>
-  </si>
-  <si>
-    <t>R 9505 PH</t>
-  </si>
-  <si>
-    <t>26/11/2005</t>
-  </si>
-  <si>
-    <t>D7244549</t>
+    <t>R 2085 GB</t>
+  </si>
+  <si>
+    <t>Supra X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -503,34 +473,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25031A6-9C77-4809-B5A1-83F15A6FEF5C}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,117 +548,59 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="G2">
-        <v>86</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
+      <c r="J2">
+        <v>1995</v>
       </c>
       <c r="K2">
         <v>1995</v>
       </c>
-      <c r="L2">
-        <v>1995</v>
+      <c r="L2" t="s">
+        <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3">
-        <v>2477</v>
-      </c>
-      <c r="H3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3">
-        <v>2005</v>
-      </c>
-      <c r="L3">
-        <v>2005</v>
-      </c>
-      <c r="M3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="O2">
+        <v>14000000</v>
+      </c>
+      <c r="P2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>